<commit_message>
Update data hotel example
Update data hotel example
</commit_message>
<xml_diff>
--- a/bin/agoda.xlsx
+++ b/bin/agoda.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\workspace\agodahome\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="9510" windowWidth="21600" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>NAME</t>
   </si>
@@ -146,44 +146,124 @@
     <t>99</t>
   </si>
   <si>
+    <t>IDs</t>
+  </si>
+  <si>
     <t>105</t>
   </si>
   <si>
-    <t>test</t>
+    <t>The Wyndham New Yorker Hotel</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>481 Eighth Avenue</t>
+  </si>
+  <si>
+    <t>8888881</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>Fitness</t>
   </si>
   <si>
     <t>106</t>
   </si>
   <si>
-    <t>ttt</t>
+    <t>Hotel Mela Times Square</t>
+  </si>
+  <si>
+    <t>120 West 44th Street</t>
+  </si>
+  <si>
+    <t>1829981</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>everything</t>
   </si>
   <si>
     <t>107</t>
   </si>
   <si>
-    <t>dddddd</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>IDs</t>
+    <t>Hotel Pennsylvania</t>
+  </si>
+  <si>
+    <t>401 7th Avenue</t>
+  </si>
+  <si>
+    <t>999999</t>
+  </si>
+  <si>
+    <t>400</t>
   </si>
   <si>
     <t>108</t>
   </si>
   <si>
-    <t>ccccc</t>
-  </si>
-  <si>
-    <t>ppppp</t>
+    <t>The Savoy Hotel</t>
+  </si>
+  <si>
+    <t>Strand, West End Soho</t>
+  </si>
+  <si>
+    <t>11233</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>Days Inn Hilton Head</t>
+  </si>
+  <si>
+    <t>hilton</t>
+  </si>
+  <si>
+    <t>9 Marina Side Drive</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Hilton Head Marriott Resort &amp; Spa</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,18 +314,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -262,10 +343,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -300,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -352,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -463,21 +544,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -494,7 +575,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -546,37 +627,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="16.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -716,124 +797,185 @@
         <v>39</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>